<commit_message>
Xây dựng ứng dụng Game “Đi tìm ẩn số”
</commit_message>
<xml_diff>
--- a/1.nen-tang-lap-trinh-java/6.Xay-dung-ung-dung-may-tinh-bo-tui.xlsx
+++ b/1.nen-tang-lap-trinh-java/6.Xay-dung-ung-dung-may-tinh-bo-tui.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\java\1.nen-tang-lap-trinh-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B0BE8A-1D7A-4150-BFE1-125A3E44F9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D90773-3E04-40C2-8D16-C5A52F80A293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30225" yWindow="1050" windowWidth="26070" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30855" yWindow="1620" windowWidth="25770" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ứng dụng máy tính bỏ túi" sheetId="1" r:id="rId1"/>
@@ -547,6 +547,122 @@
   </si>
   <si>
     <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ấ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y giá tr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ị</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> string đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ợ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c nh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ậ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p vào t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ừ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bàn phím</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
       <t>Sau khi l</t>
     </r>
     <r>
@@ -567,6 +683,304 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>y xong 1 giá tr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ị</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ậ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p vào t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ừ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bàn phím thì th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ự</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c hi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ệ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n nextLine</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>Có trên 3 tr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ờ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ợ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>p nên dùng switch đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ể</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> gi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ả</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>i quy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ế</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>t v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ấ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>n đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ề</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>Th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ự</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c thi</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>Sau khi l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ấ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>y xong các giá tr</t>
     </r>
     <r>
@@ -647,33 +1061,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>i</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ấ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>y giá tr</t>
+      <t>i. V</t>
     </r>
     <r>
       <rPr>
@@ -693,375 +1081,87 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> string đ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ợ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>c nh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ậ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p vào t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ừ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bàn phím</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>Sau khi l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ấ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>y xong 1 giá tr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ị</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> nh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ậ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p vào t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ừ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bàn phím thì th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ự</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>c hi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ệ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n nextLine</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>Có trên 3 tr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ờ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ng h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ợ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>p nên dùng switch đ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ể</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> gi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ả</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>i quy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ế</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>t v</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ấ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>n đ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ề</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>Th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>ự</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>c thi</t>
+      <t xml:space="preserve"> trí đóng cùng t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ầ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ớ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i kh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ở</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ạ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>o</t>
     </r>
     <phoneticPr fontId="2"/>
   </si>
@@ -1220,7 +1320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1231,9 +1331,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1340,6 +1437,59 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直線矢印コネクタ 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E509F452-95B0-470C-4143-2B74FC4620D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2028825" y="12982575"/>
+          <a:ext cx="19050" cy="3333750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1610,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="Q123" sqref="Q123"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1670,7 +1820,7 @@
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="4"/>
-      <c r="E10" s="10" t="s">
+      <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="5"/>
@@ -1718,163 +1868,71 @@
     </row>
     <row r="47" spans="2:12">
       <c r="B47" s="4"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="2:12">
       <c r="B48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="2:14">
       <c r="B49" s="4"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="2:14">
       <c r="B50" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="2:14">
       <c r="B51" s="4"/>
-      <c r="C51" s="11" t="s">
+      <c r="C51" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="2:14">
       <c r="B52" s="4"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11" t="s">
+      <c r="D52" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="2:14">
       <c r="B53" s="4"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11" t="s">
+      <c r="D53" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="2:14">
       <c r="B54" s="4"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11" t="s">
+      <c r="D54" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="2:14">
       <c r="B55" s="4"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11" t="s">
+      <c r="D55" t="s">
         <v>18</v>
       </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="2:14">
       <c r="B56" s="4"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="2:14">
       <c r="B57" s="4"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12" t="s">
+      <c r="D57" t="s">
         <v>53</v>
       </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
       <c r="L57" s="5"/>
       <c r="M57" t="s">
         <v>8</v>
@@ -1885,60 +1943,27 @@
     </row>
     <row r="58" spans="2:14">
       <c r="B58" s="4"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="2:14">
       <c r="B59" s="4"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11" t="s">
+      <c r="D59" t="s">
         <v>19</v>
       </c>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="2:14">
       <c r="B60" s="4"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11" t="s">
+      <c r="D60" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="2:14">
       <c r="B61" s="4"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="12" t="s">
+      <c r="D61" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
       <c r="L61" s="5"/>
       <c r="M61" t="s">
         <v>8</v>
@@ -1949,716 +1974,347 @@
     </row>
     <row r="62" spans="2:14">
       <c r="B62" s="4"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11" t="s">
+      <c r="D62" t="s">
         <v>21</v>
       </c>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
       <c r="L62" s="5"/>
       <c r="M62" t="s">
         <v>8</v>
       </c>
       <c r="N62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:14">
       <c r="B63" s="4"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="2:14">
       <c r="B64" s="4"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11" t="s">
+      <c r="D64" t="s">
         <v>22</v>
       </c>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="2:14">
       <c r="B65" s="4"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11" t="s">
+      <c r="D65" t="s">
         <v>23</v>
       </c>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="2:14">
       <c r="B66" s="4"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="12" t="s">
+      <c r="D66" t="s">
         <v>55</v>
       </c>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="2:14">
       <c r="B67" s="4"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11" t="s">
+      <c r="D67" t="s">
         <v>21</v>
       </c>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="2:14">
       <c r="B68" s="4"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="2:14">
       <c r="B69" s="4"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11" t="s">
+      <c r="D69" t="s">
         <v>24</v>
       </c>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="2:14">
       <c r="B70" s="4"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11" t="s">
+      <c r="D70" t="s">
         <v>25</v>
       </c>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="2:14">
       <c r="B71" s="4"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="12" t="s">
+      <c r="D71" t="s">
         <v>56</v>
       </c>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
       <c r="L71" s="5"/>
       <c r="M71" t="s">
         <v>8</v>
       </c>
       <c r="N71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="2:14">
       <c r="B72" s="4"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11" t="s">
+      <c r="D72" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
       <c r="L72" s="5"/>
       <c r="M72" t="s">
         <v>8</v>
       </c>
       <c r="N72" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="2:14">
       <c r="B73" s="4"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
       <c r="L73" s="5"/>
     </row>
     <row r="74" spans="2:14">
       <c r="B74" s="4"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11" t="s">
+      <c r="D74" t="s">
         <v>27</v>
       </c>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
       <c r="L74" s="5"/>
     </row>
     <row r="75" spans="2:14">
       <c r="B75" s="4"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11" t="s">
+      <c r="D75" t="s">
         <v>28</v>
       </c>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
-      <c r="K75" s="11"/>
       <c r="L75" s="5"/>
     </row>
     <row r="76" spans="2:14">
       <c r="B76" s="4"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11" t="s">
+      <c r="D76" t="s">
         <v>29</v>
       </c>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
       <c r="L76" s="5"/>
     </row>
     <row r="77" spans="2:14">
       <c r="B77" s="4"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
       <c r="L77" s="5"/>
     </row>
     <row r="78" spans="2:14">
       <c r="B78" s="4"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11" t="s">
+      <c r="D78" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="11"/>
       <c r="L78" s="5"/>
     </row>
     <row r="79" spans="2:14">
       <c r="B79" s="4"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11" t="s">
+      <c r="D79" t="s">
         <v>31</v>
       </c>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="11"/>
       <c r="L79" s="5"/>
       <c r="M79" t="s">
         <v>8</v>
       </c>
       <c r="N79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="2:14">
       <c r="B80" s="4"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11" t="s">
+      <c r="E80" t="s">
         <v>32</v>
       </c>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="11"/>
-      <c r="K80" s="11"/>
       <c r="L80" s="5"/>
     </row>
     <row r="81" spans="2:12">
       <c r="B81" s="4"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11" t="s">
+      <c r="F81" t="s">
         <v>33</v>
       </c>
-      <c r="G81" s="11" t="s">
+      <c r="G81" t="s">
         <v>34</v>
       </c>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
       <c r="L81" s="5"/>
     </row>
     <row r="82" spans="2:12">
       <c r="B82" s="4"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11" t="s">
+      <c r="F82" t="s">
         <v>35</v>
       </c>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
       <c r="L82" s="5"/>
     </row>
     <row r="83" spans="2:12">
       <c r="B83" s="4"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11" t="s">
+      <c r="E83" t="s">
         <v>36</v>
       </c>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
       <c r="L83" s="5"/>
     </row>
     <row r="84" spans="2:12">
       <c r="B84" s="4"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11" t="s">
+      <c r="F84" t="s">
         <v>33</v>
       </c>
-      <c r="G84" s="11" t="s">
+      <c r="G84" t="s">
         <v>37</v>
       </c>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
       <c r="L84" s="5"/>
     </row>
     <row r="85" spans="2:12">
       <c r="B85" s="4"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11" t="s">
+      <c r="F85" t="s">
         <v>35</v>
       </c>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="11"/>
-      <c r="K85" s="11"/>
       <c r="L85" s="5"/>
     </row>
     <row r="86" spans="2:12">
       <c r="B86" s="4"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11" t="s">
+      <c r="E86" t="s">
         <v>38</v>
       </c>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
-      <c r="K86" s="11"/>
       <c r="L86" s="5"/>
     </row>
     <row r="87" spans="2:12">
       <c r="B87" s="4"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11" t="s">
+      <c r="E87" t="s">
         <v>39</v>
       </c>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
       <c r="L87" s="5"/>
     </row>
     <row r="88" spans="2:12">
       <c r="B88" s="4"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11" t="s">
+      <c r="F88" t="s">
         <v>33</v>
       </c>
-      <c r="G88" s="11" t="s">
+      <c r="G88" t="s">
         <v>40</v>
       </c>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
       <c r="L88" s="5"/>
     </row>
     <row r="89" spans="2:12">
       <c r="B89" s="4"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11" t="s">
+      <c r="F89" t="s">
         <v>35</v>
       </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
       <c r="L89" s="5"/>
     </row>
     <row r="90" spans="2:12">
       <c r="B90" s="4"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11" t="s">
+      <c r="E90" t="s">
         <v>41</v>
       </c>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
-      <c r="K90" s="11"/>
       <c r="L90" s="5"/>
     </row>
     <row r="91" spans="2:12">
       <c r="B91" s="4"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11" t="s">
+      <c r="E91" t="s">
         <v>42</v>
       </c>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
       <c r="L91" s="5"/>
     </row>
     <row r="92" spans="2:12">
       <c r="B92" s="4"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11" t="s">
+      <c r="F92" t="s">
         <v>33</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G92" t="s">
         <v>43</v>
       </c>
-      <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
       <c r="L92" s="5"/>
     </row>
     <row r="93" spans="2:12">
       <c r="B93" s="4"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11" t="s">
+      <c r="F93" t="s">
         <v>35</v>
       </c>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="11"/>
       <c r="L93" s="5"/>
     </row>
     <row r="94" spans="2:12">
       <c r="B94" s="4"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11" t="s">
+      <c r="E94" t="s">
         <v>44</v>
       </c>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
       <c r="L94" s="5"/>
     </row>
     <row r="95" spans="2:12">
       <c r="B95" s="4"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11" t="s">
+      <c r="F95" t="s">
         <v>33</v>
       </c>
-      <c r="G95" s="11" t="s">
+      <c r="G95" t="s">
         <v>45</v>
       </c>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
       <c r="L95" s="5"/>
     </row>
     <row r="96" spans="2:12">
       <c r="B96" s="4"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11" t="s">
+      <c r="F96" t="s">
         <v>35</v>
       </c>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
       <c r="L96" s="5"/>
     </row>
     <row r="97" spans="2:12">
       <c r="B97" s="4"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
       <c r="L97" s="5"/>
     </row>
     <row r="98" spans="2:12">
       <c r="B98" s="4"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11" t="s">
+      <c r="E98" t="s">
         <v>46</v>
       </c>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
       <c r="L98" s="5"/>
     </row>
     <row r="99" spans="2:12">
       <c r="B99" s="4"/>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11" t="s">
+      <c r="F99" t="s">
         <v>33</v>
       </c>
-      <c r="G99" s="11" t="s">
+      <c r="G99" t="s">
         <v>34</v>
       </c>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
       <c r="L99" s="5"/>
     </row>
     <row r="100" spans="2:12">
       <c r="B100" s="4"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11" t="s">
+      <c r="F100" t="s">
         <v>47</v>
       </c>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
       <c r="L100" s="5"/>
     </row>
     <row r="101" spans="2:12">
       <c r="B101" s="4"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11" t="s">
+      <c r="F101" t="s">
         <v>35</v>
       </c>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="11"/>
-      <c r="K101" s="11"/>
       <c r="L101" s="5"/>
     </row>
     <row r="102" spans="2:12">
       <c r="B102" s="4"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11" t="s">
+      <c r="D102" t="s">
         <v>48</v>
       </c>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
       <c r="L102" s="5"/>
     </row>
     <row r="103" spans="2:12">
       <c r="B103" s="4"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
       <c r="L103" s="5"/>
     </row>
     <row r="104" spans="2:12">
       <c r="B104" s="4"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11" t="s">
+      <c r="D104" t="s">
         <v>49</v>
       </c>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
       <c r="L104" s="5"/>
     </row>
     <row r="105" spans="2:12">
       <c r="B105" s="4"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11" t="s">
+      <c r="D105" t="s">
         <v>50</v>
       </c>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
-      <c r="K105" s="11"/>
       <c r="L105" s="5"/>
     </row>
     <row r="106" spans="2:12">
       <c r="B106" s="4"/>
-      <c r="C106" s="11" t="s">
+      <c r="C106" t="s">
         <v>48</v>
       </c>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11"/>
       <c r="L106" s="5"/>
     </row>
     <row r="107" spans="2:12">
       <c r="B107" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="11"/>
-      <c r="K107" s="11"/>
       <c r="L107" s="5"/>
     </row>
     <row r="108" spans="2:12">
@@ -2675,8 +2331,8 @@
       <c r="L108" s="9"/>
     </row>
     <row r="111" spans="2:12">
-      <c r="B111" s="13" t="s">
-        <v>63</v>
+      <c r="B111" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -2691,158 +2347,50 @@
     </row>
     <row r="112" spans="2:12">
       <c r="B112" s="4"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="11"/>
-      <c r="H112" s="11"/>
-      <c r="I112" s="11"/>
-      <c r="J112" s="11"/>
-      <c r="K112" s="11"/>
       <c r="L112" s="5"/>
     </row>
     <row r="113" spans="2:12">
       <c r="B113" s="4"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="11"/>
-      <c r="I113" s="11"/>
-      <c r="J113" s="11"/>
-      <c r="K113" s="11"/>
       <c r="L113" s="5"/>
     </row>
     <row r="114" spans="2:12">
       <c r="B114" s="4"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
       <c r="L114" s="5"/>
     </row>
     <row r="115" spans="2:12">
       <c r="B115" s="4"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="11"/>
-      <c r="K115" s="11"/>
       <c r="L115" s="5"/>
     </row>
     <row r="116" spans="2:12">
       <c r="B116" s="4"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
-      <c r="I116" s="11"/>
-      <c r="J116" s="11"/>
-      <c r="K116" s="11"/>
       <c r="L116" s="5"/>
     </row>
     <row r="117" spans="2:12">
       <c r="B117" s="4"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
-      <c r="I117" s="11"/>
-      <c r="J117" s="11"/>
-      <c r="K117" s="11"/>
       <c r="L117" s="5"/>
     </row>
     <row r="118" spans="2:12">
       <c r="B118" s="4"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="11"/>
-      <c r="J118" s="11"/>
-      <c r="K118" s="11"/>
       <c r="L118" s="5"/>
     </row>
     <row r="119" spans="2:12">
       <c r="B119" s="4"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
-      <c r="I119" s="11"/>
-      <c r="J119" s="11"/>
-      <c r="K119" s="11"/>
       <c r="L119" s="5"/>
     </row>
     <row r="120" spans="2:12">
       <c r="B120" s="4"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
-      <c r="G120" s="11"/>
-      <c r="H120" s="11"/>
-      <c r="I120" s="11"/>
-      <c r="J120" s="11"/>
-      <c r="K120" s="11"/>
       <c r="L120" s="5"/>
     </row>
     <row r="121" spans="2:12">
       <c r="B121" s="4"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
-      <c r="G121" s="11"/>
-      <c r="H121" s="11"/>
-      <c r="I121" s="11"/>
-      <c r="J121" s="11"/>
-      <c r="K121" s="11"/>
       <c r="L121" s="5"/>
     </row>
     <row r="122" spans="2:12">
       <c r="B122" s="4"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="11"/>
-      <c r="I122" s="11"/>
-      <c r="J122" s="11"/>
-      <c r="K122" s="11"/>
       <c r="L122" s="5"/>
     </row>
     <row r="123" spans="2:12">
       <c r="B123" s="4"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="11"/>
-      <c r="I123" s="11"/>
-      <c r="J123" s="11"/>
-      <c r="K123" s="11"/>
       <c r="L123" s="5"/>
     </row>
     <row r="124" spans="2:12">

</xml_diff>